<commit_message>
Improvements in reducing execution time when launching MR jobs Introduce execution with threads for face recognition problem
</commit_message>
<xml_diff>
--- a/doc/imagenes/facerecognition-results-num-indiv.xlsx
+++ b/doc/imagenes/facerecognition-results-num-indiv.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellanzagarcia/git/ecj/doc/imagenes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="25600" windowHeight="18660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -343,12 +338,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115434944"/>
-        <c:axId val="2115648032"/>
+        <c:axId val="2124574520"/>
+        <c:axId val="2131729096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115434944"/>
+        <c:axId val="2124574520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -365,13 +361,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-ES" dirty="0" smtClean="0"/>
-                  <a:t>Número </a:t>
+                  <a:t>Número de individuos </a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="es-ES" dirty="0" smtClean="0"/>
-                  <a:t>de individuos </a:t>
-                </a:r>
-                <a:endParaRPr lang="es-ES" dirty="0" smtClean="0"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -389,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115648032"/>
+        <c:crossAx val="2131729096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -397,7 +388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115648032"/>
+        <c:axId val="2131729096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,7 +426,320 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115434944"/>
+        <c:crossAx val="2124574520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0835358553366949"/>
+          <c:y val="0.0462633451957295"/>
+          <c:w val="0.860414011852759"/>
+          <c:h val="0.781684647070362"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Secuencial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$11:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>44.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Evaluacion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$D$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2118648024"/>
+        <c:axId val="2125914344"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2118648024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" dirty="0" smtClean="0"/>
+                  <a:t>Population size (# individuals)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.630925127291951"/>
+              <c:y val="0.897419218918705"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2125914344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2125914344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" dirty="0" smtClean="0"/>
+                  <a:t>Minutes</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES" dirty="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0933966778887621"/>
+              <c:y val="0.0449940632420947"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118648024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -648,6 +952,38 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>810260</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -975,21 +1311,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:6">
       <c r="C6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:6">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1339,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:6">
       <c r="C11" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1355,7 @@
         <v>133.5</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:6">
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1369,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:6">
       <c r="C13" t="s">
         <v>2</v>
       </c>
@@ -1049,12 +1385,17 @@
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="18" spans="7:7" ht="28" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:7" ht="28">
       <c r="G18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>